<commit_message>
Fixed minor bug with padding. Updated README.
</commit_message>
<xml_diff>
--- a/stimuli/RSA_Analysis.xlsx
+++ b/stimuli/RSA_Analysis.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">a woman chopped an onion.</t>
   </si>
   <si>
-    <t xml:space="preserve">but first, she washed the onion.</t>
+    <t xml:space="preserve">but the chopped onion</t>
   </si>
   <si>
     <t xml:space="preserve">and then, she washed the onion.</t>
@@ -164,7 +164,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>